<commit_message>
feat: read and update protocols
</commit_message>
<xml_diff>
--- a/data/parameters.xlsx
+++ b/data/parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\pasa-rpa-digitacao-peg\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leand\devLeandro\mitrius\pasa\pasa-rpa-digitacao-peg\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E83CB987-FDAF-46B7-9196-D9B42E0475AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3292A75B-F7C8-4BB7-B79F-8C11C0749E3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="49080" yWindow="-120" windowWidth="19440" windowHeight="10320" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="values" sheetId="1" r:id="rId1"/>
@@ -23,23 +23,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="257">
   <si>
     <t>value</t>
   </si>
@@ -53,24 +42,9 @@
     <t>emails_success</t>
   </si>
   <si>
-    <t>https://painel.mobilesaude.com.br/login</t>
-  </si>
-  <si>
-    <t>mobilesaude.url</t>
-  </si>
-  <si>
-    <t>https://painel.mobilesaude.com.br/login/ajaxSubmitLogin</t>
-  </si>
-  <si>
-    <t>https://painel.mobilesaude.com.br/login/aplicacao/11/1</t>
-  </si>
-  <si>
     <t>https://api.mosia.chat/c1/caller/timesync/getDatetime</t>
   </si>
   <si>
-    <t>https://painel.mobilesaude.com.br/cms/reembolsoVale/listarDataTable?%s</t>
-  </si>
-  <si>
     <t>mobilesaude.bot_user_id</t>
   </si>
   <si>
@@ -95,18 +69,6 @@
     <t>benner.filial</t>
   </si>
   <si>
-    <t>https://painel.mobilesaude.com.br/cms/reembolsoVale/atribuiUsuarioReembolsoAjax</t>
-  </si>
-  <si>
-    <t>mobilesaude.atribuir</t>
-  </si>
-  <si>
-    <t>https://painel.mobilesaude.com.br/cms/reembolsoVale/editar/%s</t>
-  </si>
-  <si>
-    <t>mobilesaude.reembolso</t>
-  </si>
-  <si>
     <t>mobilesaude.bot_user_name</t>
   </si>
   <si>
@@ -179,9 +141,6 @@
     <t>mobilesaude.saude_ams_prd</t>
   </si>
   <si>
-    <t>https://painel.mobilesaude.com.br/login/aplicacao/11/</t>
-  </si>
-  <si>
     <t>mobilesaude.read_protocols_mobile_saude</t>
   </si>
   <si>
@@ -212,15 +171,6 @@
     <t>mobilesaude.worksheet</t>
   </si>
   <si>
-    <t>mobilesaude.status_filtro_prd</t>
-  </si>
-  <si>
-    <t>mobilesaude.status_filtro_hml</t>
-  </si>
-  <si>
-    <t>mobilesaude.status_final_protocolo_hml</t>
-  </si>
-  <si>
     <t>mobilesaude.assign</t>
   </si>
   <si>
@@ -260,9 +210,6 @@
     <t>Indicador true/false se o processo de atribuição de protocolos ao usuário do robô do Mobilesaúde deve ser executado</t>
   </si>
   <si>
-    <t>Link para o Mobilesaúde</t>
-  </si>
-  <si>
     <t>ID do usuário do robô no Mobilesaúde</t>
   </si>
   <si>
@@ -281,39 +228,21 @@
     <t>Link para obter o timestamp exigido pelo Mobilesaúde</t>
   </si>
   <si>
-    <t>Link para editar ou consultar um protocolo no Mobilesaúde</t>
-  </si>
-  <si>
     <t>Endpoint para atribuição de usuários no Mobilesaúde</t>
   </si>
   <si>
-    <t>Endpoint de pesquisa de protocolos no Mobilesaúde</t>
-  </si>
-  <si>
     <t>Número máximo de protocolos extraído no Mobilesaúde</t>
   </si>
   <si>
     <t>mobilesaude.alternative_user_name</t>
   </si>
   <si>
-    <t>Layla Cristina</t>
-  </si>
-  <si>
     <t>ID do usuário alternativo acionado quando houver erro no processamento do protocolo</t>
   </si>
   <si>
     <t>Nome do usuário alternativo acionado quando houver erro no processamento do protocolo</t>
   </si>
   <si>
-    <t>Id do status "solicitado" do protocolo para filtro no no Mobilesaúde de hml</t>
-  </si>
-  <si>
-    <t>Id do status "solicitado" do protocolo para filtro no no Mobilesaúde de prd</t>
-  </si>
-  <si>
-    <t>Id do status "em análise" para salvar o protocolo no no Mobilesaúde de hml</t>
-  </si>
-  <si>
     <t>Id da combobox de atribuição para o filtro de protocolos no no Mobilesaúde (2 não tribuido, 1 atribuido e 0 todos)</t>
   </si>
   <si>
@@ -401,9 +330,6 @@
     <t>card</t>
   </si>
   <si>
-    <t>RPA Python</t>
-  </si>
-  <si>
     <t>mobilesaude.assign_alternative</t>
   </si>
   <si>
@@ -464,12 +390,6 @@
     <t>Quantidade de segundos médios por execução de cada protocolo antes do robô</t>
   </si>
   <si>
-    <t>mobilesaude.status_final_protocolo_prd</t>
-  </si>
-  <si>
-    <t>Id do status "em análise" para salvar o protocolo no no Mobilesaúde de prd</t>
-  </si>
-  <si>
     <t>reembolso</t>
   </si>
   <si>
@@ -680,32 +600,213 @@
     <t>utilizador</t>
   </si>
   <si>
-    <t>prd</t>
-  </si>
-  <si>
-    <t>situação</t>
+    <t>peg_situation</t>
+  </si>
+  <si>
+    <t>peg_occurrence</t>
+  </si>
+  <si>
+    <t>refunded_value</t>
+  </si>
+  <si>
+    <t>C:\Users\leand\devLeandro\mitrius\pasa\protocolos.xlsx</t>
+  </si>
+  <si>
+    <t>mobilesaude.url_hml</t>
+  </si>
+  <si>
+    <t>https://atendente-sandbox.mosiaomnichannel.com.br/#/login</t>
+  </si>
+  <si>
+    <t>mobilesaude.url_prd</t>
+  </si>
+  <si>
+    <t>https://atendente.mosiaomnichannel.com.br/#/login</t>
+  </si>
+  <si>
+    <t>Link para o Mobilesaúde de homologação</t>
+  </si>
+  <si>
+    <t>Link para o Mobilesaúde de produção</t>
+  </si>
+  <si>
+    <t>688a1167fdb5794aae01b239</t>
+  </si>
+  <si>
+    <t>mobilesaude.attendant_status</t>
+  </si>
+  <si>
+    <t>ocupado</t>
+  </si>
+  <si>
+    <t>Status do atendente ao Logar</t>
+  </si>
+  <si>
+    <t>mobilesaude.change_attendant_status</t>
+  </si>
+  <si>
+    <t>https://api.mosiaomnichannel.com.br/privado/omni/chat/v1/gat/attendants/status</t>
+  </si>
+  <si>
+    <t>Endpoint para atribuir status do atendente ao logar</t>
+  </si>
+  <si>
+    <t>https://api.mosiaomnichannel.com.br/privado/omni/chat/v1/gat/login/atendente</t>
+  </si>
+  <si>
+    <t>https://atendente-sandbox.mosiaomnichannel.com.br/#/home/start</t>
+  </si>
+  <si>
+    <t>https://atendente.mosiaomnichannel.com.br/#/home/start</t>
+  </si>
+  <si>
+    <t>mobilesaude.form_data</t>
+  </si>
+  <si>
+    <t>https://api.mosiaomnichannel.com.br/privado/omni/form_builder/v1/gan/saudeams/form/%s/data/%s</t>
+  </si>
+  <si>
+    <t>Endpoint para buscar dados de um formulário em específico</t>
+  </si>
+  <si>
+    <t>mobilesaude.occurrence_details</t>
+  </si>
+  <si>
+    <t>https://api.mosiaomnichannel.com.br/privado/omni/ocorrencia/v1/gat/ocorrencia/detail/%s</t>
+  </si>
+  <si>
+    <t>Endpoint para pesquisa de uma ocorrência</t>
+  </si>
+  <si>
+    <t>mobilesaude_change_occurrence_status</t>
+  </si>
+  <si>
+    <t>https://api.mosiaomnichannel.com.br/privado/omni/ocorrencia/v1/gat/ocorrencia/%s/status/%s</t>
+  </si>
+  <si>
+    <t>Endpoint para alterar o status da ocorrencia</t>
+  </si>
+  <si>
+    <t>https://api.mosiaomnichannel.com.br/privado/omni/ocorrencia/v1/gat/ocorrencia</t>
+  </si>
+  <si>
+    <t>Endpoint base para buscar protocolos</t>
+  </si>
+  <si>
+    <t>mobilesaude.assigned_to_user</t>
+  </si>
+  <si>
+    <t>https://api.mosiaomnichannel.com.br/privado/omni/ocorrencia/v1/gat/ocorrencia/%s/atender</t>
+  </si>
+  <si>
+    <t>mobilesaude.get_status</t>
+  </si>
+  <si>
+    <t>https://api.mosiaomnichannel.com.br/privado/omni/ocorrencia/v1/gat/ocorrencia/tipoOcorrencia/721/status</t>
+  </si>
+  <si>
+    <t>Buscar todos os status para "Reembolso Solicitação"</t>
+  </si>
+  <si>
+    <t>mobilesaude.create_payment_data</t>
+  </si>
+  <si>
+    <t>https://api.mosiaomnichannel.com.br/privado/omni/form_builder/v1/gan/saudeams/form/%s/data</t>
+  </si>
+  <si>
+    <t>Endpoint para criar dados de pagamento</t>
+  </si>
+  <si>
+    <t>mobilesaude.env_filter_prd</t>
+  </si>
+  <si>
+    <t>Instancia da aplicação em produção</t>
+  </si>
+  <si>
+    <t>mobilesaude.env_filter_hml</t>
+  </si>
+  <si>
+    <t>Instancia da aplicação em homologação</t>
+  </si>
+  <si>
+    <t>mobilesaude.subject_filters</t>
+  </si>
+  <si>
+    <t>[673, 951]</t>
+  </si>
+  <si>
+    <t>Ids correspondente a filtro contendo Consulta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Id do status "solicitado" do protocolo para filtro no no Mobilesaúde </t>
+  </si>
+  <si>
+    <t>Id do status "em análise" do protocolo para filtro no no Mobilesaúde de hml</t>
+  </si>
+  <si>
+    <t>mobilesaude_occurrence_type_filter</t>
+  </si>
+  <si>
+    <t>ID do tipo de ocorrencia correspondente a "Reembolso e solicitação"</t>
+  </si>
+  <si>
+    <t>mobilesaude.requested_status</t>
+  </si>
+  <si>
+    <t>hml</t>
+  </si>
+  <si>
+    <t>mobilesaude.ignore</t>
+  </si>
+  <si>
+    <t>Carolina Fabri de Souza,Anthony Marcos Costa da Silva,Thais Silva de Almeida</t>
+  </si>
+  <si>
+    <t>Ignorar protocolos atribuídos para essas pessoas</t>
+  </si>
+  <si>
+    <t>valor ressarcido</t>
+  </si>
+  <si>
+    <t>situação do PEG</t>
   </si>
   <si>
     <t>ocorrência</t>
   </si>
   <si>
-    <t>peg_situation</t>
-  </si>
-  <si>
-    <t>peg_occurrence</t>
-  </si>
-  <si>
-    <t>refunded_value</t>
-  </si>
-  <si>
-    <t>valor ressarcido</t>
+    <t>mobilesaude.get_attendants</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+https://api.mosiaomnichannel.com.br/privado/omni/ocorrencia/v1/gat/ocorrencia/perfisAtendimentoPorTipoOcorrencia</t>
+  </si>
+  <si>
+    <t>Endpoint para buscar atendentes pelo tipo de ocorrência.</t>
+  </si>
+  <si>
+    <t>mobilesaude.change_occurrence</t>
+  </si>
+  <si>
+    <t>https://api.mosiaomnichannel.com.br/privado/omni/ocorrencia/v1/gat/ocorrencia/gestor/acaoEmMassa</t>
+  </si>
+  <si>
+    <t>Endpoint para realizar ações no protocolo. Ex: Mudar status e remover atendimento, atribuir a outro usuário</t>
+  </si>
+  <si>
+    <t>mobilesaude.status_analysis</t>
+  </si>
+  <si>
+    <t>Listagem Reembolso AMS</t>
+  </si>
+  <si>
+    <t>Vinicius Fiorio - Mobile Saúde</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -735,6 +836,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -757,13 +866,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" quotePrefix="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -1045,16 +1158,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C56"/>
+  <dimension ref="A1:C68"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B53" sqref="B53"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="39.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="76.5546875" customWidth="1"/>
+    <col min="2" max="2" width="97.6640625" customWidth="1"/>
     <col min="3" max="3" width="105" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1066,51 +1179,51 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>213</v>
+        <v>241</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>139</v>
+        <v>118</v>
       </c>
       <c r="B3" s="5">
         <v>180</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>140</v>
+        <v>119</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>206</v>
+        <v>183</v>
       </c>
       <c r="B4" s="4">
         <v>60000</v>
       </c>
       <c r="C4" t="s">
-        <v>205</v>
+        <v>182</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>209</v>
+        <v>186</v>
       </c>
       <c r="B5" s="4">
         <v>72</v>
       </c>
       <c r="C5" t="s">
-        <v>210</v>
+        <v>187</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -1118,10 +1231,10 @@
         <v>2</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>197</v>
+        <v>174</v>
       </c>
       <c r="C6" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -1129,571 +1242,713 @@
         <v>3</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>197</v>
+        <v>174</v>
       </c>
       <c r="C7" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="C8" t="s">
         <v>56</v>
-      </c>
-      <c r="B8" s="4"/>
-      <c r="C8" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="B9" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C9" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="B10" s="4">
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>60</v>
-      </c>
-      <c r="B11" s="4">
-        <v>1</v>
+        <v>248</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>249</v>
       </c>
       <c r="C11" t="s">
-        <v>72</v>
+        <v>250</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>5</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>4</v>
+        <v>242</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>243</v>
       </c>
       <c r="C12" t="s">
-        <v>73</v>
+        <v>244</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13">
-        <v>2995</v>
+        <v>47</v>
+      </c>
+      <c r="B13" s="4">
+        <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>22</v>
-      </c>
-      <c r="B14" t="s">
-        <v>120</v>
+        <v>194</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>195</v>
       </c>
       <c r="C14" t="s">
-        <v>75</v>
+        <v>198</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>121</v>
-      </c>
-      <c r="B15">
-        <v>0</v>
+        <v>196</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>197</v>
       </c>
       <c r="C15" t="s">
-        <v>122</v>
+        <v>199</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>64</v>
-      </c>
-      <c r="B16">
-        <v>521</v>
+        <v>5</v>
+      </c>
+      <c r="B16" t="s">
+        <v>200</v>
       </c>
       <c r="C16" t="s">
-        <v>86</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>84</v>
+        <v>13</v>
       </c>
       <c r="B17" t="s">
-        <v>85</v>
+        <v>255</v>
       </c>
       <c r="C17" t="s">
-        <v>87</v>
+        <v>61</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>11</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>6</v>
+        <v>100</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
       </c>
       <c r="C18" t="s">
-        <v>76</v>
+        <v>101</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>44</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>7</v>
+        <v>51</v>
+      </c>
+      <c r="B19">
+        <v>521</v>
       </c>
       <c r="C19" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>45</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>46</v>
+        <v>68</v>
+      </c>
+      <c r="B20" t="s">
+        <v>256</v>
       </c>
       <c r="C20" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>12</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C21" t="s">
-        <v>79</v>
+      <c r="A21" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>13</v>
+      <c r="A22" s="5" t="s">
+        <v>204</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C22" t="s">
-        <v>82</v>
+        <v>205</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>18</v>
+        <v>207</v>
       </c>
       <c r="C23" t="s">
-        <v>81</v>
+        <v>62</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>21</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>20</v>
+        <v>35</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>208</v>
       </c>
       <c r="C24" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>40</v>
-      </c>
-      <c r="B25">
-        <v>200</v>
+        <v>36</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>209</v>
       </c>
       <c r="C25" t="s">
-        <v>83</v>
+        <v>64</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>58</v>
-      </c>
-      <c r="B26">
-        <v>79</v>
+        <v>7</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="C26" t="s">
-        <v>88</v>
+        <v>65</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>57</v>
-      </c>
-      <c r="B27">
-        <v>7</v>
+        <v>210</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>211</v>
       </c>
       <c r="C27" t="s">
-        <v>89</v>
+        <v>212</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>59</v>
-      </c>
-      <c r="B28">
-        <v>82</v>
+        <v>213</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>214</v>
       </c>
       <c r="C28" t="s">
-        <v>90</v>
+        <v>215</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>141</v>
-      </c>
-      <c r="B29">
-        <v>10</v>
+        <v>216</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>217</v>
       </c>
       <c r="C29" t="s">
-        <v>142</v>
+        <v>218</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>137</v>
-      </c>
-      <c r="B30">
-        <v>0</v>
+        <v>8</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>219</v>
       </c>
       <c r="C30" t="s">
-        <v>138</v>
+        <v>220</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>23</v>
-      </c>
-      <c r="B31">
-        <v>2</v>
+        <v>221</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>222</v>
       </c>
       <c r="C31" t="s">
-        <v>91</v>
+        <v>66</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>41</v>
-      </c>
-      <c r="B32">
-        <v>1</v>
+        <v>223</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>224</v>
       </c>
       <c r="C32" t="s">
-        <v>92</v>
+        <v>225</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>42</v>
-      </c>
-      <c r="B33">
-        <v>0</v>
+        <v>251</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>252</v>
       </c>
       <c r="C33" t="s">
-        <v>93</v>
+        <v>253</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>55</v>
-      </c>
-      <c r="B34">
-        <v>1</v>
+        <v>226</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>227</v>
       </c>
       <c r="C34" t="s">
-        <v>94</v>
+        <v>228</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>117</v>
-      </c>
-      <c r="B35" t="s">
-        <v>119</v>
+        <v>229</v>
+      </c>
+      <c r="B35">
+        <v>2</v>
       </c>
       <c r="C35" t="s">
-        <v>118</v>
+        <v>230</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>49</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>14</v>
+        <v>231</v>
+      </c>
+      <c r="B36">
+        <v>1</v>
       </c>
       <c r="C36" t="s">
-        <v>95</v>
+        <v>232</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>50</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C37" t="s">
-        <v>97</v>
+      <c r="A37" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>51</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>25</v>
+        <v>31</v>
+      </c>
+      <c r="B38">
+        <v>5</v>
       </c>
       <c r="C38" t="s">
-        <v>98</v>
+        <v>67</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>112</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>111</v>
+        <v>240</v>
+      </c>
+      <c r="B39">
+        <v>1836</v>
       </c>
       <c r="C39" t="s">
-        <v>115</v>
+        <v>236</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>52</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C40" t="s">
-        <v>96</v>
+      <c r="A40" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="B40" s="5">
+        <v>721</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>53</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C41" t="s">
-        <v>99</v>
+      <c r="A41" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="B41" s="5">
+        <v>1837</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>54</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>63</v>
+        <v>116</v>
+      </c>
+      <c r="B42">
+        <v>1</v>
       </c>
       <c r="C42" t="s">
-        <v>100</v>
+        <v>117</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>113</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>114</v>
+        <v>14</v>
+      </c>
+      <c r="B43">
+        <v>2</v>
       </c>
       <c r="C43" t="s">
-        <v>116</v>
+        <v>71</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="B44">
-        <v>2025</v>
+        <v>0</v>
       </c>
       <c r="C44" t="s">
-        <v>101</v>
+        <v>72</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>17</v>
-      </c>
-      <c r="B45" t="s">
-        <v>15</v>
+        <v>33</v>
+      </c>
+      <c r="B45" s="6">
+        <v>0</v>
       </c>
       <c r="C45" t="s">
-        <v>102</v>
+        <v>73</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>24</v>
+        <v>45</v>
       </c>
       <c r="B46">
         <v>0</v>
       </c>
       <c r="C46" t="s">
-        <v>103</v>
+        <v>74</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>26</v>
-      </c>
-      <c r="B47">
-        <v>0</v>
+        <v>97</v>
+      </c>
+      <c r="B47" t="s">
+        <v>99</v>
       </c>
       <c r="C47" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>29</v>
-      </c>
-      <c r="B48" t="s">
-        <v>30</v>
+        <v>39</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="C48" t="s">
-        <v>105</v>
+        <v>75</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>32</v>
-      </c>
-      <c r="B49" t="s">
-        <v>31</v>
+        <v>40</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="C49" t="s">
-        <v>106</v>
+        <v>77</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>34</v>
-      </c>
-      <c r="B50" t="s">
-        <v>33</v>
+        <v>41</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="C50" t="s">
-        <v>107</v>
+        <v>78</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>35</v>
-      </c>
-      <c r="B51" t="s">
-        <v>36</v>
+        <v>92</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>91</v>
       </c>
       <c r="C51" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>37</v>
-      </c>
-      <c r="B52" t="s">
-        <v>123</v>
+        <v>42</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>48</v>
       </c>
       <c r="C52" t="s">
-        <v>109</v>
+        <v>76</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>38</v>
-      </c>
-      <c r="B53" t="s">
-        <v>39</v>
+        <v>43</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>49</v>
       </c>
       <c r="C53" t="s">
-        <v>110</v>
+        <v>79</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>124</v>
-      </c>
-      <c r="B54">
-        <v>1</v>
+        <v>44</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>50</v>
       </c>
       <c r="C54" t="s">
-        <v>125</v>
+        <v>80</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>135</v>
-      </c>
-      <c r="B55" t="s">
-        <v>132</v>
+        <v>93</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>94</v>
       </c>
       <c r="C55" t="s">
-        <v>136</v>
+        <v>96</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>200</v>
+        <v>11</v>
       </c>
       <c r="B56">
+        <v>2025</v>
+      </c>
+      <c r="C56" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>12</v>
+      </c>
+      <c r="B57" t="s">
+        <v>10</v>
+      </c>
+      <c r="C57" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>15</v>
+      </c>
+      <c r="B58">
+        <v>0</v>
+      </c>
+      <c r="C58" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>17</v>
+      </c>
+      <c r="B59">
+        <v>0</v>
+      </c>
+      <c r="C59" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
         <v>20</v>
       </c>
-      <c r="C56" t="s">
-        <v>201</v>
+      <c r="B60" t="s">
+        <v>21</v>
+      </c>
+      <c r="C60" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>23</v>
+      </c>
+      <c r="B61" t="s">
+        <v>22</v>
+      </c>
+      <c r="C61" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>25</v>
+      </c>
+      <c r="B62" t="s">
+        <v>24</v>
+      </c>
+      <c r="C62" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>26</v>
+      </c>
+      <c r="B63" t="s">
+        <v>27</v>
+      </c>
+      <c r="C63" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>28</v>
+      </c>
+      <c r="B64" t="s">
+        <v>102</v>
+      </c>
+      <c r="C64" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>29</v>
+      </c>
+      <c r="B65" t="s">
+        <v>30</v>
+      </c>
+      <c r="C65" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>103</v>
+      </c>
+      <c r="B66">
+        <v>1</v>
+      </c>
+      <c r="C66" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>114</v>
+      </c>
+      <c r="B67" t="s">
+        <v>111</v>
+      </c>
+      <c r="C67" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>177</v>
+      </c>
+      <c r="B68">
+        <v>20</v>
+      </c>
+      <c r="C68" t="s">
+        <v>178</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B12" r:id="rId1" xr:uid="{CD65F9E1-B2E6-43B4-82E9-6DF4A506BDFE}"/>
-    <hyperlink ref="B18" r:id="rId2" xr:uid="{126F4FEB-13DD-4FC4-AF17-532A27A19F2E}"/>
-    <hyperlink ref="B19" r:id="rId3" xr:uid="{38F5587A-B603-4B2C-9E7A-EAC1C0E30B12}"/>
-    <hyperlink ref="B21" r:id="rId4" xr:uid="{6B3BC234-FAE5-4E54-9E26-EF96D59E4C0D}"/>
-    <hyperlink ref="B22" r:id="rId5" xr:uid="{00E66A7B-31AD-47C7-A4A0-C3AECD657787}"/>
-    <hyperlink ref="B23" r:id="rId6" xr:uid="{F20B2FC9-3AE6-490E-9FC8-07609DD7A742}"/>
-    <hyperlink ref="B20" r:id="rId7" xr:uid="{CB8A04CB-EB66-40DD-A377-B43E8FBCD884}"/>
-    <hyperlink ref="B6" r:id="rId8" xr:uid="{7FE80C39-77AA-4B67-B5E1-D859B4A5E400}"/>
-    <hyperlink ref="B41" r:id="rId9" xr:uid="{C4D83FAC-8E1C-49A2-AA57-ECE0D5F8192A}"/>
-    <hyperlink ref="B42" r:id="rId10" xr:uid="{DA8F2526-9D43-4988-8A10-ACD246E21DEB}"/>
-    <hyperlink ref="B40" r:id="rId11" xr:uid="{49BD87FB-8063-4F7F-88A4-949C32E81EC2}"/>
-    <hyperlink ref="B37" r:id="rId12" xr:uid="{5EBF7E4B-683B-42A1-AE1D-BC37D003BE29}"/>
-    <hyperlink ref="B38" r:id="rId13" xr:uid="{1C4D61BD-368C-4E51-9BE6-BB20385034CE}"/>
-    <hyperlink ref="B36" r:id="rId14" xr:uid="{41870690-9729-4A3C-BA35-A842A062B531}"/>
-    <hyperlink ref="B39" r:id="rId15" xr:uid="{9B1A151E-DC26-4BFB-982B-84A42BABE47A}"/>
-    <hyperlink ref="B43" r:id="rId16" xr:uid="{ED8B71D8-70B9-4D9D-A061-7BE5F25F0286}"/>
-    <hyperlink ref="B7" r:id="rId17" xr:uid="{A39E4B9E-2E67-4651-877E-D770F6BF49BE}"/>
+    <hyperlink ref="B6" r:id="rId1" xr:uid="{7FE80C39-77AA-4B67-B5E1-D859B4A5E400}"/>
+    <hyperlink ref="B53" r:id="rId2" xr:uid="{C4D83FAC-8E1C-49A2-AA57-ECE0D5F8192A}"/>
+    <hyperlink ref="B54" r:id="rId3" xr:uid="{DA8F2526-9D43-4988-8A10-ACD246E21DEB}"/>
+    <hyperlink ref="B52" r:id="rId4" xr:uid="{49BD87FB-8063-4F7F-88A4-949C32E81EC2}"/>
+    <hyperlink ref="B49" r:id="rId5" xr:uid="{5EBF7E4B-683B-42A1-AE1D-BC37D003BE29}"/>
+    <hyperlink ref="B50" r:id="rId6" xr:uid="{1C4D61BD-368C-4E51-9BE6-BB20385034CE}"/>
+    <hyperlink ref="B48" r:id="rId7" xr:uid="{41870690-9729-4A3C-BA35-A842A062B531}"/>
+    <hyperlink ref="B51" r:id="rId8" xr:uid="{9B1A151E-DC26-4BFB-982B-84A42BABE47A}"/>
+    <hyperlink ref="B55" r:id="rId9" xr:uid="{ED8B71D8-70B9-4D9D-A061-7BE5F25F0286}"/>
+    <hyperlink ref="B7" r:id="rId10" xr:uid="{A39E4B9E-2E67-4651-877E-D770F6BF49BE}"/>
+    <hyperlink ref="B15" r:id="rId11" location="/login" xr:uid="{B1878979-8DDB-45DA-94DB-BEFD37231B5E}"/>
+    <hyperlink ref="B14" r:id="rId12" location="/login" xr:uid="{BD5F0F1E-2089-49FE-91FA-6C1E643B36C9}"/>
+    <hyperlink ref="B23" r:id="rId13" xr:uid="{09FB775C-78B9-4C50-A9F6-16CAF8B18285}"/>
+    <hyperlink ref="B24" r:id="rId14" location="/home/start" xr:uid="{3B9C2C0E-248B-425B-939B-3C41D4F09735}"/>
+    <hyperlink ref="B26" r:id="rId15" xr:uid="{A1EE6531-7664-42F4-9EC4-12E967C86AE4}"/>
+    <hyperlink ref="B30" r:id="rId16" xr:uid="{716BCCC0-2D41-4155-ABF7-A106E0FFB4D0}"/>
+    <hyperlink ref="B31" r:id="rId17" xr:uid="{0E2F51F3-7F97-4776-985C-32A5A420B28D}"/>
+    <hyperlink ref="B25" r:id="rId18" location="/home/start" xr:uid="{72EB0A52-ED09-4F6A-915A-BCD23C02BE80}"/>
+    <hyperlink ref="B22" r:id="rId19" xr:uid="{2B7B9775-38A0-4A04-8786-F837731EEA1B}"/>
+    <hyperlink ref="B28" r:id="rId20" xr:uid="{0B0D0069-F21D-4F07-BE36-68E4F09B997E}"/>
+    <hyperlink ref="B27" r:id="rId21" xr:uid="{DB320590-BB5A-4B32-AB47-42CDA50AEB31}"/>
+    <hyperlink ref="B29" r:id="rId22" xr:uid="{FB4CD2A5-4466-4D0A-B529-5507E411CB4B}"/>
+    <hyperlink ref="B32" r:id="rId23" xr:uid="{D16CA40F-AE6E-4CB1-8D7D-ACC5DD4BC5D6}"/>
+    <hyperlink ref="B11" r:id="rId24" display="https://api.mosiaomnichannel.com.br/privado/omni/ocorrencia/v1/gat/ocorrencia/perfilAtendenteStatus" xr:uid="{45A70590-7D02-4F0C-92C9-9545F7636DC8}"/>
+    <hyperlink ref="B33" r:id="rId25" xr:uid="{6B9291C1-A8FB-4011-A859-56D575C62630}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId18"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId26"/>
 </worksheet>
 </file>
 
@@ -1713,42 +1968,42 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>133</v>
+        <v>112</v>
       </c>
       <c r="B1" t="s">
-        <v>134</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>126</v>
+        <v>105</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>127</v>
+        <v>106</v>
       </c>
       <c r="B3" t="s">
-        <v>128</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>129</v>
+        <v>108</v>
       </c>
       <c r="B4" t="s">
-        <v>130</v>
+        <v>109</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>131</v>
+        <v>110</v>
       </c>
       <c r="B5" t="s">
-        <v>132</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -1760,8 +2015,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE612074-01A7-422D-8EA3-A30E57C47C51}">
   <dimension ref="A1:A36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27:A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1771,182 +2026,182 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>202</v>
+        <v>179</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>203</v>
+        <v>180</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>143</v>
+        <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>144</v>
+        <v>121</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>145</v>
+        <v>122</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>146</v>
+        <v>123</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>147</v>
+        <v>124</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>148</v>
+        <v>125</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>149</v>
+        <v>126</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>150</v>
+        <v>127</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>151</v>
+        <v>128</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>212</v>
+        <v>189</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>152</v>
+        <v>129</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>153</v>
+        <v>130</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>154</v>
+        <v>131</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>155</v>
+        <v>132</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>156</v>
+        <v>133</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>157</v>
+        <v>134</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>158</v>
+        <v>135</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>159</v>
+        <v>136</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>160</v>
+        <v>137</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>161</v>
+        <v>138</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>162</v>
+        <v>139</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>163</v>
+        <v>140</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>164</v>
+        <v>141</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>165</v>
+        <v>142</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>166</v>
+        <v>143</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>199</v>
+        <v>144</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>167</v>
+        <v>147</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>170</v>
+        <v>145</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>168</v>
+        <v>176</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>214</v>
+        <v>245</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>219</v>
+        <v>246</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>169</v>
+        <v>247</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>215</v>
+        <v>146</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>208</v>
+        <v>185</v>
       </c>
     </row>
   </sheetData>
@@ -1958,8 +2213,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45D36061-0536-447A-B9AE-F657ED82A38A}">
   <dimension ref="A1:A36"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1969,182 +2224,182 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>204</v>
+        <v>181</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>171</v>
+        <v>148</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>172</v>
+        <v>149</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>173</v>
+        <v>150</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>174</v>
+        <v>151</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>175</v>
+        <v>152</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>176</v>
+        <v>153</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>177</v>
+        <v>154</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>178</v>
+        <v>155</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>119</v>
+        <v>99</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>211</v>
+        <v>188</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>179</v>
+        <v>156</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>180</v>
+        <v>157</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>181</v>
+        <v>158</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>182</v>
+        <v>159</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>183</v>
+        <v>160</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>184</v>
+        <v>161</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>185</v>
+        <v>162</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>186</v>
+        <v>163</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>187</v>
+        <v>164</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>188</v>
+        <v>165</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>189</v>
+        <v>166</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>190</v>
+        <v>167</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>191</v>
+        <v>168</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>192</v>
+        <v>169</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>193</v>
+        <v>170</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>198</v>
+        <v>144</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>194</v>
+        <v>172</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>195</v>
+        <v>175</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>216</v>
+        <v>192</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>218</v>
+        <v>190</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>217</v>
+        <v>173</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>207</v>
+        <v>184</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
chore: reorganize project folders
</commit_message>
<xml_diff>
--- a/data/parameters.xlsx
+++ b/data/parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leand\devLeandro\mitrius\pasa\pasa-rpa-digitacao-peg\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3292A75B-F7C8-4BB7-B79F-8C11C0749E3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE3AA5CC-3708-4B20-BCFD-C56E343289FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="values" sheetId="1" r:id="rId1"/>
@@ -1160,18 +1160,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="97.6640625" customWidth="1"/>
+    <col min="1" max="1" width="39.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="97.7109375" customWidth="1"/>
     <col min="3" max="3" width="105" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1182,7 +1182,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>34</v>
       </c>
@@ -1193,7 +1193,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>118</v>
       </c>
@@ -1204,7 +1204,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>183</v>
       </c>
@@ -1215,7 +1215,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>186</v>
       </c>
@@ -1226,7 +1226,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -1237,7 +1237,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -1248,7 +1248,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>46</v>
       </c>
@@ -1259,29 +1259,29 @@
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>37</v>
       </c>
       <c r="B9" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C9" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>38</v>
       </c>
       <c r="B10" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C10" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>248</v>
       </c>
@@ -1292,7 +1292,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>242</v>
       </c>
@@ -1303,7 +1303,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>47</v>
       </c>
@@ -1314,7 +1314,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>194</v>
       </c>
@@ -1325,7 +1325,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>196</v>
       </c>
@@ -1336,7 +1336,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>5</v>
       </c>
@@ -1347,7 +1347,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>13</v>
       </c>
@@ -1358,7 +1358,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>100</v>
       </c>
@@ -1369,7 +1369,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>51</v>
       </c>
@@ -1380,7 +1380,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>68</v>
       </c>
@@ -1391,7 +1391,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>201</v>
       </c>
@@ -1402,7 +1402,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>204</v>
       </c>
@@ -1413,7 +1413,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>6</v>
       </c>
@@ -1424,7 +1424,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>35</v>
       </c>
@@ -1435,7 +1435,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>36</v>
       </c>
@@ -1446,7 +1446,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>7</v>
       </c>
@@ -1457,7 +1457,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>210</v>
       </c>
@@ -1468,7 +1468,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>213</v>
       </c>
@@ -1479,7 +1479,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>216</v>
       </c>
@@ -1490,7 +1490,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>8</v>
       </c>
@@ -1501,7 +1501,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>221</v>
       </c>
@@ -1512,7 +1512,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>223</v>
       </c>
@@ -1523,7 +1523,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>251</v>
       </c>
@@ -1534,7 +1534,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>226</v>
       </c>
@@ -1545,7 +1545,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>229</v>
       </c>
@@ -1556,7 +1556,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>231</v>
       </c>
@@ -1567,7 +1567,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
         <v>233</v>
       </c>
@@ -1578,7 +1578,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>31</v>
       </c>
@@ -1589,7 +1589,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>240</v>
       </c>
@@ -1600,7 +1600,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
         <v>238</v>
       </c>
@@ -1611,7 +1611,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
         <v>254</v>
       </c>
@@ -1622,7 +1622,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>116</v>
       </c>
@@ -1633,7 +1633,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>14</v>
       </c>
@@ -1644,7 +1644,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>32</v>
       </c>
@@ -1655,7 +1655,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>33</v>
       </c>
@@ -1666,7 +1666,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>45</v>
       </c>
@@ -1677,7 +1677,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>97</v>
       </c>
@@ -1688,7 +1688,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>39</v>
       </c>
@@ -1699,7 +1699,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>40</v>
       </c>
@@ -1710,7 +1710,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>41</v>
       </c>
@@ -1721,7 +1721,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>92</v>
       </c>
@@ -1732,7 +1732,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>42</v>
       </c>
@@ -1743,7 +1743,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>43</v>
       </c>
@@ -1754,7 +1754,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>44</v>
       </c>
@@ -1765,7 +1765,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>93</v>
       </c>
@@ -1776,7 +1776,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>11</v>
       </c>
@@ -1787,7 +1787,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>12</v>
       </c>
@@ -1798,7 +1798,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>15</v>
       </c>
@@ -1809,7 +1809,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>17</v>
       </c>
@@ -1820,7 +1820,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>20</v>
       </c>
@@ -1831,7 +1831,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>23</v>
       </c>
@@ -1842,7 +1842,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>25</v>
       </c>
@@ -1853,7 +1853,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>26</v>
       </c>
@@ -1864,7 +1864,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>28</v>
       </c>
@@ -1875,7 +1875,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>29</v>
       </c>
@@ -1886,7 +1886,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>103</v>
       </c>
@@ -1897,7 +1897,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>114</v>
       </c>
@@ -1908,7 +1908,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>177</v>
       </c>
@@ -1960,13 +1960,13 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="66.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="66.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>112</v>
       </c>
@@ -1974,7 +1974,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>105</v>
       </c>
@@ -1982,7 +1982,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>106</v>
       </c>
@@ -1990,7 +1990,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>108</v>
       </c>
@@ -1998,7 +1998,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>110</v>
       </c>
@@ -2019,187 +2019,187 @@
       <selection activeCell="A27" sqref="A27:A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>185</v>
       </c>
@@ -2217,187 +2217,187 @@
       <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>184</v>
       </c>

</xml_diff>